<commit_message>
Add more info to AWS PLF
</commit_message>
<xml_diff>
--- a/Marketplace/LANSA Scalable License/AWS/2016-08-24.xlsx
+++ b/Marketplace/LANSA Scalable License/AWS/2016-08-24.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert.SYD\Documents\GitHub\cookbooks_scalable\Marketplace\LANSA Scalable License\AWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31540EB2-B4F9-4739-A084-52B2F07F9766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" tabRatio="421" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11760" tabRatio="421" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="12" r:id="rId1"/>
@@ -32,7 +33,7 @@
     <definedName name="TRUE_FALSE">Validation_Data!$A$2:$A$3</definedName>
     <definedName name="Users_Units">Validation_Data!$L$2</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1848,7 +1849,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -4589,415 +4590,415 @@
     <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
     <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
     <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Akzent1" xfId="42"/>
-    <cellStyle name="20% - Akzent1 10" xfId="43"/>
-    <cellStyle name="20% - Akzent1 11" xfId="44"/>
-    <cellStyle name="20% - Akzent1 12" xfId="45"/>
-    <cellStyle name="20% - Akzent1 13" xfId="46"/>
-    <cellStyle name="20% - Akzent1 14" xfId="47"/>
-    <cellStyle name="20% - Akzent1 15" xfId="48"/>
-    <cellStyle name="20% - Akzent1 16" xfId="49"/>
-    <cellStyle name="20% - Akzent1 17" xfId="50"/>
-    <cellStyle name="20% - Akzent1 2" xfId="51"/>
-    <cellStyle name="20% - Akzent1 3" xfId="52"/>
-    <cellStyle name="20% - Akzent1 4" xfId="53"/>
-    <cellStyle name="20% - Akzent1 5" xfId="54"/>
-    <cellStyle name="20% - Akzent1 6" xfId="55"/>
-    <cellStyle name="20% - Akzent1 7" xfId="56"/>
-    <cellStyle name="20% - Akzent1 8" xfId="57"/>
-    <cellStyle name="20% - Akzent1 9" xfId="58"/>
-    <cellStyle name="20% - Akzent1_International Settings" xfId="59"/>
-    <cellStyle name="20% - Akzent2" xfId="60"/>
-    <cellStyle name="20% - Akzent2 10" xfId="61"/>
-    <cellStyle name="20% - Akzent2 11" xfId="62"/>
-    <cellStyle name="20% - Akzent2 12" xfId="63"/>
-    <cellStyle name="20% - Akzent2 13" xfId="64"/>
-    <cellStyle name="20% - Akzent2 14" xfId="65"/>
-    <cellStyle name="20% - Akzent2 15" xfId="66"/>
-    <cellStyle name="20% - Akzent2 16" xfId="67"/>
-    <cellStyle name="20% - Akzent2 17" xfId="68"/>
-    <cellStyle name="20% - Akzent2 2" xfId="69"/>
-    <cellStyle name="20% - Akzent2 3" xfId="70"/>
-    <cellStyle name="20% - Akzent2 4" xfId="71"/>
-    <cellStyle name="20% - Akzent2 5" xfId="72"/>
-    <cellStyle name="20% - Akzent2 6" xfId="73"/>
-    <cellStyle name="20% - Akzent2 7" xfId="74"/>
-    <cellStyle name="20% - Akzent2 8" xfId="75"/>
-    <cellStyle name="20% - Akzent2 9" xfId="76"/>
-    <cellStyle name="20% - Akzent2_International Settings" xfId="77"/>
-    <cellStyle name="20% - Akzent3" xfId="78"/>
-    <cellStyle name="20% - Akzent3 10" xfId="79"/>
-    <cellStyle name="20% - Akzent3 11" xfId="80"/>
-    <cellStyle name="20% - Akzent3 12" xfId="81"/>
-    <cellStyle name="20% - Akzent3 13" xfId="82"/>
-    <cellStyle name="20% - Akzent3 14" xfId="83"/>
-    <cellStyle name="20% - Akzent3 15" xfId="84"/>
-    <cellStyle name="20% - Akzent3 16" xfId="85"/>
-    <cellStyle name="20% - Akzent3 17" xfId="86"/>
-    <cellStyle name="20% - Akzent3 2" xfId="87"/>
-    <cellStyle name="20% - Akzent3 3" xfId="88"/>
-    <cellStyle name="20% - Akzent3 4" xfId="89"/>
-    <cellStyle name="20% - Akzent3 5" xfId="90"/>
-    <cellStyle name="20% - Akzent3 6" xfId="91"/>
-    <cellStyle name="20% - Akzent3 7" xfId="92"/>
-    <cellStyle name="20% - Akzent3 8" xfId="93"/>
-    <cellStyle name="20% - Akzent3 9" xfId="94"/>
-    <cellStyle name="20% - Akzent3_International Settings" xfId="95"/>
-    <cellStyle name="20% - Akzent4" xfId="96"/>
-    <cellStyle name="20% - Akzent4 10" xfId="97"/>
-    <cellStyle name="20% - Akzent4 11" xfId="98"/>
-    <cellStyle name="20% - Akzent4 12" xfId="99"/>
-    <cellStyle name="20% - Akzent4 13" xfId="100"/>
-    <cellStyle name="20% - Akzent4 14" xfId="101"/>
-    <cellStyle name="20% - Akzent4 15" xfId="102"/>
-    <cellStyle name="20% - Akzent4 16" xfId="103"/>
-    <cellStyle name="20% - Akzent4 17" xfId="104"/>
-    <cellStyle name="20% - Akzent4 2" xfId="105"/>
-    <cellStyle name="20% - Akzent4 3" xfId="106"/>
-    <cellStyle name="20% - Akzent4 4" xfId="107"/>
-    <cellStyle name="20% - Akzent4 5" xfId="108"/>
-    <cellStyle name="20% - Akzent4 6" xfId="109"/>
-    <cellStyle name="20% - Akzent4 7" xfId="110"/>
-    <cellStyle name="20% - Akzent4 8" xfId="111"/>
-    <cellStyle name="20% - Akzent4 9" xfId="112"/>
-    <cellStyle name="20% - Akzent4_International Settings" xfId="113"/>
-    <cellStyle name="20% - Akzent5" xfId="114"/>
-    <cellStyle name="20% - Akzent5 10" xfId="115"/>
-    <cellStyle name="20% - Akzent5 11" xfId="116"/>
-    <cellStyle name="20% - Akzent5 12" xfId="117"/>
-    <cellStyle name="20% - Akzent5 13" xfId="118"/>
-    <cellStyle name="20% - Akzent5 14" xfId="119"/>
-    <cellStyle name="20% - Akzent5 15" xfId="120"/>
-    <cellStyle name="20% - Akzent5 16" xfId="121"/>
-    <cellStyle name="20% - Akzent5 17" xfId="122"/>
-    <cellStyle name="20% - Akzent5 2" xfId="123"/>
-    <cellStyle name="20% - Akzent5 3" xfId="124"/>
-    <cellStyle name="20% - Akzent5 4" xfId="125"/>
-    <cellStyle name="20% - Akzent5 5" xfId="126"/>
-    <cellStyle name="20% - Akzent5 6" xfId="127"/>
-    <cellStyle name="20% - Akzent5 7" xfId="128"/>
-    <cellStyle name="20% - Akzent5 8" xfId="129"/>
-    <cellStyle name="20% - Akzent5 9" xfId="130"/>
-    <cellStyle name="20% - Akzent5_International Settings" xfId="131"/>
-    <cellStyle name="20% - Akzent6" xfId="132"/>
-    <cellStyle name="20% - Akzent6 10" xfId="133"/>
-    <cellStyle name="20% - Akzent6 11" xfId="134"/>
-    <cellStyle name="20% - Akzent6 12" xfId="135"/>
-    <cellStyle name="20% - Akzent6 13" xfId="136"/>
-    <cellStyle name="20% - Akzent6 14" xfId="137"/>
-    <cellStyle name="20% - Akzent6 15" xfId="138"/>
-    <cellStyle name="20% - Akzent6 16" xfId="139"/>
-    <cellStyle name="20% - Akzent6 17" xfId="140"/>
-    <cellStyle name="20% - Akzent6 2" xfId="141"/>
-    <cellStyle name="20% - Akzent6 3" xfId="142"/>
-    <cellStyle name="20% - Akzent6 4" xfId="143"/>
-    <cellStyle name="20% - Akzent6 5" xfId="144"/>
-    <cellStyle name="20% - Akzent6 6" xfId="145"/>
-    <cellStyle name="20% - Akzent6 7" xfId="146"/>
-    <cellStyle name="20% - Akzent6 8" xfId="147"/>
-    <cellStyle name="20% - Akzent6 9" xfId="148"/>
-    <cellStyle name="20% - Akzent6_International Settings" xfId="149"/>
-    <cellStyle name="20% - アクセント 1" xfId="150"/>
-    <cellStyle name="20% - アクセント 2" xfId="151"/>
-    <cellStyle name="20% - アクセント 3" xfId="152"/>
-    <cellStyle name="20% - アクセント 4" xfId="153"/>
-    <cellStyle name="20% - アクセント 5" xfId="154"/>
-    <cellStyle name="20% - アクセント 6" xfId="155"/>
+    <cellStyle name="20% - Akzent1" xfId="42" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - Akzent1 10" xfId="43" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - Akzent1 11" xfId="44" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - Akzent1 12" xfId="45" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - Akzent1 13" xfId="46" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - Akzent1 14" xfId="47" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - Akzent1 15" xfId="48" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="20% - Akzent1 16" xfId="49" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - Akzent1 17" xfId="50" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - Akzent1 2" xfId="51" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20% - Akzent1 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - Akzent1 4" xfId="53" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="20% - Akzent1 5" xfId="54" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="20% - Akzent1 6" xfId="55" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - Akzent1 7" xfId="56" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="20% - Akzent1 8" xfId="57" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="20% - Akzent1 9" xfId="58" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="20% - Akzent1_International Settings" xfId="59" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="20% - Akzent2" xfId="60" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="20% - Akzent2 10" xfId="61" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="20% - Akzent2 11" xfId="62" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="20% - Akzent2 12" xfId="63" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="20% - Akzent2 13" xfId="64" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="20% - Akzent2 14" xfId="65" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - Akzent2 15" xfId="66" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="20% - Akzent2 16" xfId="67" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="20% - Akzent2 17" xfId="68" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="20% - Akzent2 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="20% - Akzent2 3" xfId="70" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="20% - Akzent2 4" xfId="71" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - Akzent2 5" xfId="72" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="20% - Akzent2 6" xfId="73" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="20% - Akzent2 7" xfId="74" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="20% - Akzent2 8" xfId="75" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="20% - Akzent2 9" xfId="76" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="20% - Akzent2_International Settings" xfId="77" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="20% - Akzent3" xfId="78" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="20% - Akzent3 10" xfId="79" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="20% - Akzent3 11" xfId="80" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="20% - Akzent3 12" xfId="81" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="20% - Akzent3 13" xfId="82" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="20% - Akzent3 14" xfId="83" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="20% - Akzent3 15" xfId="84" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="20% - Akzent3 16" xfId="85" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="20% - Akzent3 17" xfId="86" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="20% - Akzent3 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="20% - Akzent3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="20% - Akzent3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="20% - Akzent3 5" xfId="90" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="20% - Akzent3 6" xfId="91" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="20% - Akzent3 7" xfId="92" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="20% - Akzent3 8" xfId="93" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="20% - Akzent3 9" xfId="94" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="20% - Akzent3_International Settings" xfId="95" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="20% - Akzent4" xfId="96" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="20% - Akzent4 10" xfId="97" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="20% - Akzent4 11" xfId="98" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="20% - Akzent4 12" xfId="99" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="20% - Akzent4 13" xfId="100" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="20% - Akzent4 14" xfId="101" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="20% - Akzent4 15" xfId="102" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="20% - Akzent4 16" xfId="103" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="20% - Akzent4 17" xfId="104" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="20% - Akzent4 2" xfId="105" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="20% - Akzent4 3" xfId="106" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="20% - Akzent4 4" xfId="107" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="20% - Akzent4 5" xfId="108" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="20% - Akzent4 6" xfId="109" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="20% - Akzent4 7" xfId="110" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="20% - Akzent4 8" xfId="111" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="20% - Akzent4 9" xfId="112" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="20% - Akzent4_International Settings" xfId="113" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="20% - Akzent5" xfId="114" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="20% - Akzent5 10" xfId="115" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="20% - Akzent5 11" xfId="116" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="20% - Akzent5 12" xfId="117" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="20% - Akzent5 13" xfId="118" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="20% - Akzent5 14" xfId="119" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="20% - Akzent5 15" xfId="120" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="20% - Akzent5 16" xfId="121" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="20% - Akzent5 17" xfId="122" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="20% - Akzent5 2" xfId="123" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="20% - Akzent5 3" xfId="124" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="20% - Akzent5 4" xfId="125" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="20% - Akzent5 5" xfId="126" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="20% - Akzent5 6" xfId="127" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="20% - Akzent5 7" xfId="128" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="20% - Akzent5 8" xfId="129" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="20% - Akzent5 9" xfId="130" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="20% - Akzent5_International Settings" xfId="131" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="20% - Akzent6" xfId="132" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="20% - Akzent6 10" xfId="133" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="20% - Akzent6 11" xfId="134" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="20% - Akzent6 12" xfId="135" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="20% - Akzent6 13" xfId="136" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="20% - Akzent6 14" xfId="137" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="20% - Akzent6 15" xfId="138" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="20% - Akzent6 16" xfId="139" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="20% - Akzent6 17" xfId="140" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="20% - Akzent6 2" xfId="141" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="20% - Akzent6 3" xfId="142" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="20% - Akzent6 4" xfId="143" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="20% - Akzent6 5" xfId="144" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="20% - Akzent6 6" xfId="145" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="20% - Akzent6 7" xfId="146" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="20% - Akzent6 8" xfId="147" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="20% - Akzent6 9" xfId="148" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="20% - Akzent6_International Settings" xfId="149" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="20% - アクセント 1" xfId="150" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="20% - アクセント 2" xfId="151" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="20% - アクセント 3" xfId="152" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="20% - アクセント 4" xfId="153" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="20% - アクセント 5" xfId="154" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="20% - アクセント 6" xfId="155" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
     <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
     <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Akzent1" xfId="156"/>
-    <cellStyle name="40% - Akzent1 10" xfId="157"/>
-    <cellStyle name="40% - Akzent1 11" xfId="158"/>
-    <cellStyle name="40% - Akzent1 12" xfId="159"/>
-    <cellStyle name="40% - Akzent1 13" xfId="160"/>
-    <cellStyle name="40% - Akzent1 14" xfId="161"/>
-    <cellStyle name="40% - Akzent1 15" xfId="162"/>
-    <cellStyle name="40% - Akzent1 16" xfId="163"/>
-    <cellStyle name="40% - Akzent1 17" xfId="164"/>
-    <cellStyle name="40% - Akzent1 2" xfId="165"/>
-    <cellStyle name="40% - Akzent1 3" xfId="166"/>
-    <cellStyle name="40% - Akzent1 4" xfId="167"/>
-    <cellStyle name="40% - Akzent1 5" xfId="168"/>
-    <cellStyle name="40% - Akzent1 6" xfId="169"/>
-    <cellStyle name="40% - Akzent1 7" xfId="170"/>
-    <cellStyle name="40% - Akzent1 8" xfId="171"/>
-    <cellStyle name="40% - Akzent1 9" xfId="172"/>
-    <cellStyle name="40% - Akzent1_International Settings" xfId="173"/>
-    <cellStyle name="40% - Akzent2" xfId="174"/>
-    <cellStyle name="40% - Akzent2 10" xfId="175"/>
-    <cellStyle name="40% - Akzent2 11" xfId="176"/>
-    <cellStyle name="40% - Akzent2 12" xfId="177"/>
-    <cellStyle name="40% - Akzent2 13" xfId="178"/>
-    <cellStyle name="40% - Akzent2 14" xfId="179"/>
-    <cellStyle name="40% - Akzent2 15" xfId="180"/>
-    <cellStyle name="40% - Akzent2 16" xfId="181"/>
-    <cellStyle name="40% - Akzent2 17" xfId="182"/>
-    <cellStyle name="40% - Akzent2 2" xfId="183"/>
-    <cellStyle name="40% - Akzent2 3" xfId="184"/>
-    <cellStyle name="40% - Akzent2 4" xfId="185"/>
-    <cellStyle name="40% - Akzent2 5" xfId="186"/>
-    <cellStyle name="40% - Akzent2 6" xfId="187"/>
-    <cellStyle name="40% - Akzent2 7" xfId="188"/>
-    <cellStyle name="40% - Akzent2 8" xfId="189"/>
-    <cellStyle name="40% - Akzent2 9" xfId="190"/>
-    <cellStyle name="40% - Akzent2_International Settings" xfId="191"/>
-    <cellStyle name="40% - Akzent3" xfId="192"/>
-    <cellStyle name="40% - Akzent3 10" xfId="193"/>
-    <cellStyle name="40% - Akzent3 11" xfId="194"/>
-    <cellStyle name="40% - Akzent3 12" xfId="195"/>
-    <cellStyle name="40% - Akzent3 13" xfId="196"/>
-    <cellStyle name="40% - Akzent3 14" xfId="197"/>
-    <cellStyle name="40% - Akzent3 15" xfId="198"/>
-    <cellStyle name="40% - Akzent3 16" xfId="199"/>
-    <cellStyle name="40% - Akzent3 17" xfId="200"/>
-    <cellStyle name="40% - Akzent3 2" xfId="201"/>
-    <cellStyle name="40% - Akzent3 3" xfId="202"/>
-    <cellStyle name="40% - Akzent3 4" xfId="203"/>
-    <cellStyle name="40% - Akzent3 5" xfId="204"/>
-    <cellStyle name="40% - Akzent3 6" xfId="205"/>
-    <cellStyle name="40% - Akzent3 7" xfId="206"/>
-    <cellStyle name="40% - Akzent3 8" xfId="207"/>
-    <cellStyle name="40% - Akzent3 9" xfId="208"/>
-    <cellStyle name="40% - Akzent3_International Settings" xfId="209"/>
-    <cellStyle name="40% - Akzent4" xfId="210"/>
-    <cellStyle name="40% - Akzent4 10" xfId="211"/>
-    <cellStyle name="40% - Akzent4 11" xfId="212"/>
-    <cellStyle name="40% - Akzent4 12" xfId="213"/>
-    <cellStyle name="40% - Akzent4 13" xfId="214"/>
-    <cellStyle name="40% - Akzent4 14" xfId="215"/>
-    <cellStyle name="40% - Akzent4 15" xfId="216"/>
-    <cellStyle name="40% - Akzent4 16" xfId="217"/>
-    <cellStyle name="40% - Akzent4 17" xfId="218"/>
-    <cellStyle name="40% - Akzent4 2" xfId="219"/>
-    <cellStyle name="40% - Akzent4 3" xfId="220"/>
-    <cellStyle name="40% - Akzent4 4" xfId="221"/>
-    <cellStyle name="40% - Akzent4 5" xfId="222"/>
-    <cellStyle name="40% - Akzent4 6" xfId="223"/>
-    <cellStyle name="40% - Akzent4 7" xfId="224"/>
-    <cellStyle name="40% - Akzent4 8" xfId="225"/>
-    <cellStyle name="40% - Akzent4 9" xfId="226"/>
-    <cellStyle name="40% - Akzent4_International Settings" xfId="227"/>
-    <cellStyle name="40% - Akzent5" xfId="228"/>
-    <cellStyle name="40% - Akzent5 10" xfId="229"/>
-    <cellStyle name="40% - Akzent5 11" xfId="230"/>
-    <cellStyle name="40% - Akzent5 12" xfId="231"/>
-    <cellStyle name="40% - Akzent5 13" xfId="232"/>
-    <cellStyle name="40% - Akzent5 14" xfId="233"/>
-    <cellStyle name="40% - Akzent5 15" xfId="234"/>
-    <cellStyle name="40% - Akzent5 16" xfId="235"/>
-    <cellStyle name="40% - Akzent5 17" xfId="236"/>
-    <cellStyle name="40% - Akzent5 2" xfId="237"/>
-    <cellStyle name="40% - Akzent5 3" xfId="238"/>
-    <cellStyle name="40% - Akzent5 4" xfId="239"/>
-    <cellStyle name="40% - Akzent5 5" xfId="240"/>
-    <cellStyle name="40% - Akzent5 6" xfId="241"/>
-    <cellStyle name="40% - Akzent5 7" xfId="242"/>
-    <cellStyle name="40% - Akzent5 8" xfId="243"/>
-    <cellStyle name="40% - Akzent5 9" xfId="244"/>
-    <cellStyle name="40% - Akzent5_International Settings" xfId="245"/>
-    <cellStyle name="40% - Akzent6" xfId="246"/>
-    <cellStyle name="40% - Akzent6 10" xfId="247"/>
-    <cellStyle name="40% - Akzent6 11" xfId="248"/>
-    <cellStyle name="40% - Akzent6 12" xfId="249"/>
-    <cellStyle name="40% - Akzent6 13" xfId="250"/>
-    <cellStyle name="40% - Akzent6 14" xfId="251"/>
-    <cellStyle name="40% - Akzent6 15" xfId="252"/>
-    <cellStyle name="40% - Akzent6 16" xfId="253"/>
-    <cellStyle name="40% - Akzent6 17" xfId="254"/>
-    <cellStyle name="40% - Akzent6 2" xfId="255"/>
-    <cellStyle name="40% - Akzent6 3" xfId="256"/>
-    <cellStyle name="40% - Akzent6 4" xfId="257"/>
-    <cellStyle name="40% - Akzent6 5" xfId="258"/>
-    <cellStyle name="40% - Akzent6 6" xfId="259"/>
-    <cellStyle name="40% - Akzent6 7" xfId="260"/>
-    <cellStyle name="40% - Akzent6 8" xfId="261"/>
-    <cellStyle name="40% - Akzent6 9" xfId="262"/>
-    <cellStyle name="40% - Akzent6_International Settings" xfId="263"/>
-    <cellStyle name="40% - アクセント 1" xfId="264"/>
-    <cellStyle name="40% - アクセント 2" xfId="265"/>
-    <cellStyle name="40% - アクセント 3" xfId="266"/>
-    <cellStyle name="40% - アクセント 4" xfId="267"/>
-    <cellStyle name="40% - アクセント 5" xfId="268"/>
-    <cellStyle name="40% - アクセント 6" xfId="269"/>
+    <cellStyle name="40% - Akzent1" xfId="156" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="40% - Akzent1 10" xfId="157" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="40% - Akzent1 11" xfId="158" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="40% - Akzent1 12" xfId="159" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="40% - Akzent1 13" xfId="160" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="40% - Akzent1 14" xfId="161" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="40% - Akzent1 15" xfId="162" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="40% - Akzent1 16" xfId="163" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="40% - Akzent1 17" xfId="164" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="40% - Akzent1 2" xfId="165" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="40% - Akzent1 3" xfId="166" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="40% - Akzent1 4" xfId="167" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="40% - Akzent1 5" xfId="168" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="40% - Akzent1 6" xfId="169" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="40% - Akzent1 7" xfId="170" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="40% - Akzent1 8" xfId="171" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="40% - Akzent1 9" xfId="172" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="40% - Akzent1_International Settings" xfId="173" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="40% - Akzent2" xfId="174" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="40% - Akzent2 10" xfId="175" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="40% - Akzent2 11" xfId="176" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="40% - Akzent2 12" xfId="177" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="40% - Akzent2 13" xfId="178" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="40% - Akzent2 14" xfId="179" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="40% - Akzent2 15" xfId="180" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="40% - Akzent2 16" xfId="181" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="40% - Akzent2 17" xfId="182" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="40% - Akzent2 2" xfId="183" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="40% - Akzent2 3" xfId="184" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="40% - Akzent2 4" xfId="185" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="40% - Akzent2 5" xfId="186" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="40% - Akzent2 6" xfId="187" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="40% - Akzent2 7" xfId="188" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="40% - Akzent2 8" xfId="189" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="40% - Akzent2 9" xfId="190" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="40% - Akzent2_International Settings" xfId="191" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="40% - Akzent3" xfId="192" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="40% - Akzent3 10" xfId="193" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="40% - Akzent3 11" xfId="194" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="40% - Akzent3 12" xfId="195" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="40% - Akzent3 13" xfId="196" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="40% - Akzent3 14" xfId="197" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="40% - Akzent3 15" xfId="198" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="40% - Akzent3 16" xfId="199" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="40% - Akzent3 17" xfId="200" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="40% - Akzent3 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="40% - Akzent3 3" xfId="202" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="40% - Akzent3 4" xfId="203" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="40% - Akzent3 5" xfId="204" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
+    <cellStyle name="40% - Akzent3 6" xfId="205" xr:uid="{00000000-0005-0000-0000-0000AF000000}"/>
+    <cellStyle name="40% - Akzent3 7" xfId="206" xr:uid="{00000000-0005-0000-0000-0000B0000000}"/>
+    <cellStyle name="40% - Akzent3 8" xfId="207" xr:uid="{00000000-0005-0000-0000-0000B1000000}"/>
+    <cellStyle name="40% - Akzent3 9" xfId="208" xr:uid="{00000000-0005-0000-0000-0000B2000000}"/>
+    <cellStyle name="40% - Akzent3_International Settings" xfId="209" xr:uid="{00000000-0005-0000-0000-0000B3000000}"/>
+    <cellStyle name="40% - Akzent4" xfId="210" xr:uid="{00000000-0005-0000-0000-0000B4000000}"/>
+    <cellStyle name="40% - Akzent4 10" xfId="211" xr:uid="{00000000-0005-0000-0000-0000B5000000}"/>
+    <cellStyle name="40% - Akzent4 11" xfId="212" xr:uid="{00000000-0005-0000-0000-0000B6000000}"/>
+    <cellStyle name="40% - Akzent4 12" xfId="213" xr:uid="{00000000-0005-0000-0000-0000B7000000}"/>
+    <cellStyle name="40% - Akzent4 13" xfId="214" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
+    <cellStyle name="40% - Akzent4 14" xfId="215" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
+    <cellStyle name="40% - Akzent4 15" xfId="216" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
+    <cellStyle name="40% - Akzent4 16" xfId="217" xr:uid="{00000000-0005-0000-0000-0000BB000000}"/>
+    <cellStyle name="40% - Akzent4 17" xfId="218" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
+    <cellStyle name="40% - Akzent4 2" xfId="219" xr:uid="{00000000-0005-0000-0000-0000BD000000}"/>
+    <cellStyle name="40% - Akzent4 3" xfId="220" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
+    <cellStyle name="40% - Akzent4 4" xfId="221" xr:uid="{00000000-0005-0000-0000-0000BF000000}"/>
+    <cellStyle name="40% - Akzent4 5" xfId="222" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
+    <cellStyle name="40% - Akzent4 6" xfId="223" xr:uid="{00000000-0005-0000-0000-0000C1000000}"/>
+    <cellStyle name="40% - Akzent4 7" xfId="224" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
+    <cellStyle name="40% - Akzent4 8" xfId="225" xr:uid="{00000000-0005-0000-0000-0000C3000000}"/>
+    <cellStyle name="40% - Akzent4 9" xfId="226" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
+    <cellStyle name="40% - Akzent4_International Settings" xfId="227" xr:uid="{00000000-0005-0000-0000-0000C5000000}"/>
+    <cellStyle name="40% - Akzent5" xfId="228" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
+    <cellStyle name="40% - Akzent5 10" xfId="229" xr:uid="{00000000-0005-0000-0000-0000C7000000}"/>
+    <cellStyle name="40% - Akzent5 11" xfId="230" xr:uid="{00000000-0005-0000-0000-0000C8000000}"/>
+    <cellStyle name="40% - Akzent5 12" xfId="231" xr:uid="{00000000-0005-0000-0000-0000C9000000}"/>
+    <cellStyle name="40% - Akzent5 13" xfId="232" xr:uid="{00000000-0005-0000-0000-0000CA000000}"/>
+    <cellStyle name="40% - Akzent5 14" xfId="233" xr:uid="{00000000-0005-0000-0000-0000CB000000}"/>
+    <cellStyle name="40% - Akzent5 15" xfId="234" xr:uid="{00000000-0005-0000-0000-0000CC000000}"/>
+    <cellStyle name="40% - Akzent5 16" xfId="235" xr:uid="{00000000-0005-0000-0000-0000CD000000}"/>
+    <cellStyle name="40% - Akzent5 17" xfId="236" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
+    <cellStyle name="40% - Akzent5 2" xfId="237" xr:uid="{00000000-0005-0000-0000-0000CF000000}"/>
+    <cellStyle name="40% - Akzent5 3" xfId="238" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
+    <cellStyle name="40% - Akzent5 4" xfId="239" xr:uid="{00000000-0005-0000-0000-0000D1000000}"/>
+    <cellStyle name="40% - Akzent5 5" xfId="240" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
+    <cellStyle name="40% - Akzent5 6" xfId="241" xr:uid="{00000000-0005-0000-0000-0000D3000000}"/>
+    <cellStyle name="40% - Akzent5 7" xfId="242" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
+    <cellStyle name="40% - Akzent5 8" xfId="243" xr:uid="{00000000-0005-0000-0000-0000D5000000}"/>
+    <cellStyle name="40% - Akzent5 9" xfId="244" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
+    <cellStyle name="40% - Akzent5_International Settings" xfId="245" xr:uid="{00000000-0005-0000-0000-0000D7000000}"/>
+    <cellStyle name="40% - Akzent6" xfId="246" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
+    <cellStyle name="40% - Akzent6 10" xfId="247" xr:uid="{00000000-0005-0000-0000-0000D9000000}"/>
+    <cellStyle name="40% - Akzent6 11" xfId="248" xr:uid="{00000000-0005-0000-0000-0000DA000000}"/>
+    <cellStyle name="40% - Akzent6 12" xfId="249" xr:uid="{00000000-0005-0000-0000-0000DB000000}"/>
+    <cellStyle name="40% - Akzent6 13" xfId="250" xr:uid="{00000000-0005-0000-0000-0000DC000000}"/>
+    <cellStyle name="40% - Akzent6 14" xfId="251" xr:uid="{00000000-0005-0000-0000-0000DD000000}"/>
+    <cellStyle name="40% - Akzent6 15" xfId="252" xr:uid="{00000000-0005-0000-0000-0000DE000000}"/>
+    <cellStyle name="40% - Akzent6 16" xfId="253" xr:uid="{00000000-0005-0000-0000-0000DF000000}"/>
+    <cellStyle name="40% - Akzent6 17" xfId="254" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
+    <cellStyle name="40% - Akzent6 2" xfId="255" xr:uid="{00000000-0005-0000-0000-0000E1000000}"/>
+    <cellStyle name="40% - Akzent6 3" xfId="256" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
+    <cellStyle name="40% - Akzent6 4" xfId="257" xr:uid="{00000000-0005-0000-0000-0000E3000000}"/>
+    <cellStyle name="40% - Akzent6 5" xfId="258" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
+    <cellStyle name="40% - Akzent6 6" xfId="259" xr:uid="{00000000-0005-0000-0000-0000E5000000}"/>
+    <cellStyle name="40% - Akzent6 7" xfId="260" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
+    <cellStyle name="40% - Akzent6 8" xfId="261" xr:uid="{00000000-0005-0000-0000-0000E7000000}"/>
+    <cellStyle name="40% - Akzent6 9" xfId="262" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
+    <cellStyle name="40% - Akzent6_International Settings" xfId="263" xr:uid="{00000000-0005-0000-0000-0000E9000000}"/>
+    <cellStyle name="40% - アクセント 1" xfId="264" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="40% - アクセント 2" xfId="265" xr:uid="{00000000-0005-0000-0000-0000EB000000}"/>
+    <cellStyle name="40% - アクセント 3" xfId="266" xr:uid="{00000000-0005-0000-0000-0000EC000000}"/>
+    <cellStyle name="40% - アクセント 4" xfId="267" xr:uid="{00000000-0005-0000-0000-0000ED000000}"/>
+    <cellStyle name="40% - アクセント 5" xfId="268" xr:uid="{00000000-0005-0000-0000-0000EE000000}"/>
+    <cellStyle name="40% - アクセント 6" xfId="269" xr:uid="{00000000-0005-0000-0000-0000EF000000}"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="60% - Akzent1" xfId="270"/>
-    <cellStyle name="60% - Akzent2" xfId="271"/>
-    <cellStyle name="60% - Akzent3" xfId="272"/>
-    <cellStyle name="60% - Akzent4" xfId="273"/>
-    <cellStyle name="60% - Akzent5" xfId="274"/>
-    <cellStyle name="60% - Akzent6" xfId="275"/>
-    <cellStyle name="60% - アクセント 1" xfId="276"/>
-    <cellStyle name="60% - アクセント 2" xfId="277"/>
-    <cellStyle name="60% - アクセント 3" xfId="278"/>
-    <cellStyle name="60% - アクセント 4" xfId="279"/>
-    <cellStyle name="60% - アクセント 5" xfId="280"/>
-    <cellStyle name="60% - アクセント 6" xfId="281"/>
+    <cellStyle name="60% - Akzent1" xfId="270" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="60% - Akzent2" xfId="271" xr:uid="{00000000-0005-0000-0000-0000F7000000}"/>
+    <cellStyle name="60% - Akzent3" xfId="272" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="60% - Akzent4" xfId="273" xr:uid="{00000000-0005-0000-0000-0000F9000000}"/>
+    <cellStyle name="60% - Akzent5" xfId="274" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="60% - Akzent6" xfId="275" xr:uid="{00000000-0005-0000-0000-0000FB000000}"/>
+    <cellStyle name="60% - アクセント 1" xfId="276" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
+    <cellStyle name="60% - アクセント 2" xfId="277" xr:uid="{00000000-0005-0000-0000-0000FD000000}"/>
+    <cellStyle name="60% - アクセント 3" xfId="278" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
+    <cellStyle name="60% - アクセント 4" xfId="279" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
+    <cellStyle name="60% - アクセント 5" xfId="280" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
+    <cellStyle name="60% - アクセント 6" xfId="281" xr:uid="{00000000-0005-0000-0000-000001010000}"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="282"/>
-    <cellStyle name="Akzent2" xfId="283"/>
-    <cellStyle name="Akzent3" xfId="284"/>
-    <cellStyle name="Akzent4" xfId="285"/>
-    <cellStyle name="Akzent5" xfId="286"/>
-    <cellStyle name="Akzent6" xfId="287"/>
-    <cellStyle name="Ausgabe" xfId="288"/>
+    <cellStyle name="Akzent1" xfId="282" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Akzent2" xfId="283" xr:uid="{00000000-0005-0000-0000-000009010000}"/>
+    <cellStyle name="Akzent3" xfId="284" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
+    <cellStyle name="Akzent4" xfId="285" xr:uid="{00000000-0005-0000-0000-00000B010000}"/>
+    <cellStyle name="Akzent5" xfId="286" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
+    <cellStyle name="Akzent6" xfId="287" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
+    <cellStyle name="Ausgabe" xfId="288" xr:uid="{00000000-0005-0000-0000-00000E010000}"/>
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="289"/>
+    <cellStyle name="Berechnung" xfId="289" xr:uid="{00000000-0005-0000-0000-000010010000}"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma [0] 2" xfId="290"/>
-    <cellStyle name="Comma 2" xfId="291"/>
-    <cellStyle name="Currency [0] 2" xfId="292"/>
-    <cellStyle name="Eingabe" xfId="293"/>
-    <cellStyle name="Ergebnis" xfId="294"/>
-    <cellStyle name="Erklärender Text" xfId="295"/>
+    <cellStyle name="Comma [0] 2" xfId="290" xr:uid="{00000000-0005-0000-0000-000013010000}"/>
+    <cellStyle name="Comma 2" xfId="291" xr:uid="{00000000-0005-0000-0000-000014010000}"/>
+    <cellStyle name="Currency [0] 2" xfId="292" xr:uid="{00000000-0005-0000-0000-000015010000}"/>
+    <cellStyle name="Eingabe" xfId="293" xr:uid="{00000000-0005-0000-0000-000016010000}"/>
+    <cellStyle name="Ergebnis" xfId="294" xr:uid="{00000000-0005-0000-0000-000017010000}"/>
+    <cellStyle name="Erklärender Text" xfId="295" xr:uid="{00000000-0005-0000-0000-000018010000}"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="296"/>
+    <cellStyle name="Gut" xfId="296" xr:uid="{00000000-0005-0000-0000-00001B010000}"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Hyperlink" xfId="414" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="298"/>
-    <cellStyle name="Hyperlink 2 2" xfId="299"/>
-    <cellStyle name="Hyperlink 2 3" xfId="300"/>
-    <cellStyle name="Hyperlink 2 4" xfId="301"/>
-    <cellStyle name="Hyperlink 2 5" xfId="302"/>
-    <cellStyle name="Hyperlink 3" xfId="303"/>
-    <cellStyle name="Hyperlink 3 2" xfId="304"/>
-    <cellStyle name="Hyperlink 3 3" xfId="305"/>
-    <cellStyle name="Hyperlink 4" xfId="306"/>
-    <cellStyle name="Hyperlink 4 2" xfId="307"/>
-    <cellStyle name="Hyperlink 4 3" xfId="308"/>
-    <cellStyle name="Hyperlink 5" xfId="309"/>
-    <cellStyle name="Hyperlink 5 2" xfId="310"/>
-    <cellStyle name="Hyperlink 5 3" xfId="311"/>
-    <cellStyle name="Hyperlink 5 4" xfId="312"/>
-    <cellStyle name="Hyperlink 5 5" xfId="313"/>
-    <cellStyle name="Hyperlink 6" xfId="314"/>
-    <cellStyle name="Hyperlink 7" xfId="315"/>
-    <cellStyle name="Hyperlink 8" xfId="297"/>
+    <cellStyle name="Hyperlink 2" xfId="298" xr:uid="{00000000-0005-0000-0000-000021010000}"/>
+    <cellStyle name="Hyperlink 2 2" xfId="299" xr:uid="{00000000-0005-0000-0000-000022010000}"/>
+    <cellStyle name="Hyperlink 2 3" xfId="300" xr:uid="{00000000-0005-0000-0000-000023010000}"/>
+    <cellStyle name="Hyperlink 2 4" xfId="301" xr:uid="{00000000-0005-0000-0000-000024010000}"/>
+    <cellStyle name="Hyperlink 2 5" xfId="302" xr:uid="{00000000-0005-0000-0000-000025010000}"/>
+    <cellStyle name="Hyperlink 3" xfId="303" xr:uid="{00000000-0005-0000-0000-000026010000}"/>
+    <cellStyle name="Hyperlink 3 2" xfId="304" xr:uid="{00000000-0005-0000-0000-000027010000}"/>
+    <cellStyle name="Hyperlink 3 3" xfId="305" xr:uid="{00000000-0005-0000-0000-000028010000}"/>
+    <cellStyle name="Hyperlink 4" xfId="306" xr:uid="{00000000-0005-0000-0000-000029010000}"/>
+    <cellStyle name="Hyperlink 4 2" xfId="307" xr:uid="{00000000-0005-0000-0000-00002A010000}"/>
+    <cellStyle name="Hyperlink 4 3" xfId="308" xr:uid="{00000000-0005-0000-0000-00002B010000}"/>
+    <cellStyle name="Hyperlink 5" xfId="309" xr:uid="{00000000-0005-0000-0000-00002C010000}"/>
+    <cellStyle name="Hyperlink 5 2" xfId="310" xr:uid="{00000000-0005-0000-0000-00002D010000}"/>
+    <cellStyle name="Hyperlink 5 3" xfId="311" xr:uid="{00000000-0005-0000-0000-00002E010000}"/>
+    <cellStyle name="Hyperlink 5 4" xfId="312" xr:uid="{00000000-0005-0000-0000-00002F010000}"/>
+    <cellStyle name="Hyperlink 5 5" xfId="313" xr:uid="{00000000-0005-0000-0000-000030010000}"/>
+    <cellStyle name="Hyperlink 6" xfId="314" xr:uid="{00000000-0005-0000-0000-000031010000}"/>
+    <cellStyle name="Hyperlink 7" xfId="315" xr:uid="{00000000-0005-0000-0000-000032010000}"/>
+    <cellStyle name="Hyperlink 8" xfId="297" xr:uid="{00000000-0005-0000-0000-000033010000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10 2" xfId="316"/>
-    <cellStyle name="Normal 11 2" xfId="317"/>
-    <cellStyle name="Normal 13" xfId="318"/>
-    <cellStyle name="Normal 16" xfId="319"/>
-    <cellStyle name="Normal 16 2" xfId="320"/>
-    <cellStyle name="Normal 16_International Settings" xfId="321"/>
-    <cellStyle name="Normal 2" xfId="322"/>
-    <cellStyle name="Normal 2 2" xfId="323"/>
-    <cellStyle name="Normal 2 3" xfId="324"/>
-    <cellStyle name="Normal 2 3 2" xfId="325"/>
-    <cellStyle name="Normal 2 3 2 2" xfId="326"/>
-    <cellStyle name="Normal 2 3 2_International Settings" xfId="327"/>
-    <cellStyle name="Normal 2 3 3" xfId="328"/>
-    <cellStyle name="Normal 2 3_International Settings" xfId="329"/>
-    <cellStyle name="Normal 2_SourceWorkbook" xfId="330"/>
-    <cellStyle name="Normal 3" xfId="331"/>
-    <cellStyle name="Normal 3 2" xfId="332"/>
-    <cellStyle name="Normal 3 2 2" xfId="333"/>
-    <cellStyle name="Normal 3 2_International Settings" xfId="334"/>
-    <cellStyle name="Normal 3_International Settings" xfId="335"/>
-    <cellStyle name="Normal 4" xfId="336"/>
-    <cellStyle name="Normal 4 10" xfId="337"/>
-    <cellStyle name="Normal 4 11" xfId="338"/>
-    <cellStyle name="Normal 4 2" xfId="339"/>
-    <cellStyle name="Normal 4 2 2" xfId="340"/>
-    <cellStyle name="Normal 4 2 3" xfId="341"/>
-    <cellStyle name="Normal 4 2_International Settings" xfId="342"/>
-    <cellStyle name="Normal 4 3" xfId="343"/>
-    <cellStyle name="Normal 4 4" xfId="344"/>
-    <cellStyle name="Normal 4 5" xfId="345"/>
-    <cellStyle name="Normal 4 6" xfId="346"/>
-    <cellStyle name="Normal 4 7" xfId="347"/>
-    <cellStyle name="Normal 4 8" xfId="348"/>
-    <cellStyle name="Normal 4 9" xfId="349"/>
-    <cellStyle name="Normal 4_International Settings" xfId="350"/>
-    <cellStyle name="Normal 5" xfId="351"/>
-    <cellStyle name="Normal 5 2" xfId="352"/>
-    <cellStyle name="Normal 6" xfId="353"/>
-    <cellStyle name="Normal 6 2" xfId="354"/>
-    <cellStyle name="Normal 6 3" xfId="355"/>
-    <cellStyle name="Normal 6 4" xfId="356"/>
-    <cellStyle name="Normal 6 5" xfId="357"/>
-    <cellStyle name="Normal 6 6" xfId="358"/>
-    <cellStyle name="Normal 6_SourceWorkbook" xfId="359"/>
-    <cellStyle name="Normal 7" xfId="360"/>
-    <cellStyle name="Normal 7 2" xfId="361"/>
-    <cellStyle name="Normal 7 3" xfId="362"/>
-    <cellStyle name="Normal 7 4" xfId="363"/>
-    <cellStyle name="Normal 7 5" xfId="364"/>
-    <cellStyle name="Normal 7 6" xfId="365"/>
-    <cellStyle name="Normal 7 7" xfId="366"/>
-    <cellStyle name="Normal 8" xfId="367"/>
-    <cellStyle name="Normal 8 2" xfId="368"/>
-    <cellStyle name="Normal 9" xfId="369"/>
-    <cellStyle name="Normal 9 2" xfId="370"/>
+    <cellStyle name="Normal 10 2" xfId="316" xr:uid="{00000000-0005-0000-0000-000038010000}"/>
+    <cellStyle name="Normal 11 2" xfId="317" xr:uid="{00000000-0005-0000-0000-000039010000}"/>
+    <cellStyle name="Normal 13" xfId="318" xr:uid="{00000000-0005-0000-0000-00003A010000}"/>
+    <cellStyle name="Normal 16" xfId="319" xr:uid="{00000000-0005-0000-0000-00003B010000}"/>
+    <cellStyle name="Normal 16 2" xfId="320" xr:uid="{00000000-0005-0000-0000-00003C010000}"/>
+    <cellStyle name="Normal 16_International Settings" xfId="321" xr:uid="{00000000-0005-0000-0000-00003D010000}"/>
+    <cellStyle name="Normal 2" xfId="322" xr:uid="{00000000-0005-0000-0000-00003E010000}"/>
+    <cellStyle name="Normal 2 2" xfId="323" xr:uid="{00000000-0005-0000-0000-00003F010000}"/>
+    <cellStyle name="Normal 2 3" xfId="324" xr:uid="{00000000-0005-0000-0000-000040010000}"/>
+    <cellStyle name="Normal 2 3 2" xfId="325" xr:uid="{00000000-0005-0000-0000-000041010000}"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="326" xr:uid="{00000000-0005-0000-0000-000042010000}"/>
+    <cellStyle name="Normal 2 3 2_International Settings" xfId="327" xr:uid="{00000000-0005-0000-0000-000043010000}"/>
+    <cellStyle name="Normal 2 3 3" xfId="328" xr:uid="{00000000-0005-0000-0000-000044010000}"/>
+    <cellStyle name="Normal 2 3_International Settings" xfId="329" xr:uid="{00000000-0005-0000-0000-000045010000}"/>
+    <cellStyle name="Normal 2_SourceWorkbook" xfId="330" xr:uid="{00000000-0005-0000-0000-000046010000}"/>
+    <cellStyle name="Normal 3" xfId="331" xr:uid="{00000000-0005-0000-0000-000047010000}"/>
+    <cellStyle name="Normal 3 2" xfId="332" xr:uid="{00000000-0005-0000-0000-000048010000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="333" xr:uid="{00000000-0005-0000-0000-000049010000}"/>
+    <cellStyle name="Normal 3 2_International Settings" xfId="334" xr:uid="{00000000-0005-0000-0000-00004A010000}"/>
+    <cellStyle name="Normal 3_International Settings" xfId="335" xr:uid="{00000000-0005-0000-0000-00004B010000}"/>
+    <cellStyle name="Normal 4" xfId="336" xr:uid="{00000000-0005-0000-0000-00004C010000}"/>
+    <cellStyle name="Normal 4 10" xfId="337" xr:uid="{00000000-0005-0000-0000-00004D010000}"/>
+    <cellStyle name="Normal 4 11" xfId="338" xr:uid="{00000000-0005-0000-0000-00004E010000}"/>
+    <cellStyle name="Normal 4 2" xfId="339" xr:uid="{00000000-0005-0000-0000-00004F010000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="340" xr:uid="{00000000-0005-0000-0000-000050010000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="341" xr:uid="{00000000-0005-0000-0000-000051010000}"/>
+    <cellStyle name="Normal 4 2_International Settings" xfId="342" xr:uid="{00000000-0005-0000-0000-000052010000}"/>
+    <cellStyle name="Normal 4 3" xfId="343" xr:uid="{00000000-0005-0000-0000-000053010000}"/>
+    <cellStyle name="Normal 4 4" xfId="344" xr:uid="{00000000-0005-0000-0000-000054010000}"/>
+    <cellStyle name="Normal 4 5" xfId="345" xr:uid="{00000000-0005-0000-0000-000055010000}"/>
+    <cellStyle name="Normal 4 6" xfId="346" xr:uid="{00000000-0005-0000-0000-000056010000}"/>
+    <cellStyle name="Normal 4 7" xfId="347" xr:uid="{00000000-0005-0000-0000-000057010000}"/>
+    <cellStyle name="Normal 4 8" xfId="348" xr:uid="{00000000-0005-0000-0000-000058010000}"/>
+    <cellStyle name="Normal 4 9" xfId="349" xr:uid="{00000000-0005-0000-0000-000059010000}"/>
+    <cellStyle name="Normal 4_International Settings" xfId="350" xr:uid="{00000000-0005-0000-0000-00005A010000}"/>
+    <cellStyle name="Normal 5" xfId="351" xr:uid="{00000000-0005-0000-0000-00005B010000}"/>
+    <cellStyle name="Normal 5 2" xfId="352" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
+    <cellStyle name="Normal 6" xfId="353" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
+    <cellStyle name="Normal 6 2" xfId="354" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
+    <cellStyle name="Normal 6 3" xfId="355" xr:uid="{00000000-0005-0000-0000-00005F010000}"/>
+    <cellStyle name="Normal 6 4" xfId="356" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
+    <cellStyle name="Normal 6 5" xfId="357" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
+    <cellStyle name="Normal 6 6" xfId="358" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
+    <cellStyle name="Normal 6_SourceWorkbook" xfId="359" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
+    <cellStyle name="Normal 7" xfId="360" xr:uid="{00000000-0005-0000-0000-000064010000}"/>
+    <cellStyle name="Normal 7 2" xfId="361" xr:uid="{00000000-0005-0000-0000-000065010000}"/>
+    <cellStyle name="Normal 7 3" xfId="362" xr:uid="{00000000-0005-0000-0000-000066010000}"/>
+    <cellStyle name="Normal 7 4" xfId="363" xr:uid="{00000000-0005-0000-0000-000067010000}"/>
+    <cellStyle name="Normal 7 5" xfId="364" xr:uid="{00000000-0005-0000-0000-000068010000}"/>
+    <cellStyle name="Normal 7 6" xfId="365" xr:uid="{00000000-0005-0000-0000-000069010000}"/>
+    <cellStyle name="Normal 7 7" xfId="366" xr:uid="{00000000-0005-0000-0000-00006A010000}"/>
+    <cellStyle name="Normal 8" xfId="367" xr:uid="{00000000-0005-0000-0000-00006B010000}"/>
+    <cellStyle name="Normal 8 2" xfId="368" xr:uid="{00000000-0005-0000-0000-00006C010000}"/>
+    <cellStyle name="Normal 9" xfId="369" xr:uid="{00000000-0005-0000-0000-00006D010000}"/>
+    <cellStyle name="Normal 9 2" xfId="370" xr:uid="{00000000-0005-0000-0000-00006E010000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="371"/>
+    <cellStyle name="Notiz" xfId="371" xr:uid="{00000000-0005-0000-0000-000070010000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="372"/>
-    <cellStyle name="Standard 2" xfId="373"/>
-    <cellStyle name="Standard 3" xfId="374"/>
-    <cellStyle name="Standard 4" xfId="375"/>
-    <cellStyle name="Standard 4 2" xfId="376"/>
-    <cellStyle name="Standard 4 3" xfId="377"/>
-    <cellStyle name="Standard 4_International Settings" xfId="378"/>
-    <cellStyle name="Standard 5" xfId="379"/>
-    <cellStyle name="Style 1" xfId="380"/>
+    <cellStyle name="Schlecht" xfId="372" xr:uid="{00000000-0005-0000-0000-000072010000}"/>
+    <cellStyle name="Standard 2" xfId="373" xr:uid="{00000000-0005-0000-0000-000073010000}"/>
+    <cellStyle name="Standard 3" xfId="374" xr:uid="{00000000-0005-0000-0000-000074010000}"/>
+    <cellStyle name="Standard 4" xfId="375" xr:uid="{00000000-0005-0000-0000-000075010000}"/>
+    <cellStyle name="Standard 4 2" xfId="376" xr:uid="{00000000-0005-0000-0000-000076010000}"/>
+    <cellStyle name="Standard 4 3" xfId="377" xr:uid="{00000000-0005-0000-0000-000077010000}"/>
+    <cellStyle name="Standard 4_International Settings" xfId="378" xr:uid="{00000000-0005-0000-0000-000078010000}"/>
+    <cellStyle name="Standard 5" xfId="379" xr:uid="{00000000-0005-0000-0000-000079010000}"/>
+    <cellStyle name="Style 1" xfId="380" xr:uid="{00000000-0005-0000-0000-00007A010000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Überschrift" xfId="381"/>
-    <cellStyle name="Überschrift 1" xfId="382"/>
-    <cellStyle name="Überschrift 2" xfId="383"/>
-    <cellStyle name="Überschrift 3" xfId="384"/>
-    <cellStyle name="Überschrift 4" xfId="385"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="386"/>
-    <cellStyle name="Warnender Text" xfId="387"/>
+    <cellStyle name="Überschrift" xfId="381" xr:uid="{00000000-0005-0000-0000-00007D010000}"/>
+    <cellStyle name="Überschrift 1" xfId="382" xr:uid="{00000000-0005-0000-0000-00007E010000}"/>
+    <cellStyle name="Überschrift 2" xfId="383" xr:uid="{00000000-0005-0000-0000-00007F010000}"/>
+    <cellStyle name="Überschrift 3" xfId="384" xr:uid="{00000000-0005-0000-0000-000080010000}"/>
+    <cellStyle name="Überschrift 4" xfId="385" xr:uid="{00000000-0005-0000-0000-000081010000}"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="386" xr:uid="{00000000-0005-0000-0000-000082010000}"/>
+    <cellStyle name="Warnender Text" xfId="387" xr:uid="{00000000-0005-0000-0000-000083010000}"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="388"/>
-    <cellStyle name="アクセント 1" xfId="389"/>
-    <cellStyle name="アクセント 2" xfId="390"/>
-    <cellStyle name="アクセント 3" xfId="391"/>
-    <cellStyle name="アクセント 4" xfId="392"/>
-    <cellStyle name="アクセント 5" xfId="393"/>
-    <cellStyle name="アクセント 6" xfId="394"/>
-    <cellStyle name="タイトル" xfId="395"/>
-    <cellStyle name="チェック セル" xfId="396"/>
-    <cellStyle name="どちらでもない" xfId="397"/>
-    <cellStyle name="メモ" xfId="398"/>
-    <cellStyle name="リンク セル" xfId="399"/>
-    <cellStyle name="入力" xfId="400"/>
-    <cellStyle name="出力" xfId="401"/>
-    <cellStyle name="悪い" xfId="402"/>
-    <cellStyle name="標準_Data Definitions" xfId="403"/>
-    <cellStyle name="良い" xfId="404"/>
-    <cellStyle name="見出し 1" xfId="405"/>
-    <cellStyle name="見出し 2" xfId="406"/>
-    <cellStyle name="見出し 3" xfId="407"/>
-    <cellStyle name="見出し 4" xfId="408"/>
-    <cellStyle name="計算" xfId="409"/>
-    <cellStyle name="説明文" xfId="410"/>
-    <cellStyle name="警告文" xfId="411"/>
-    <cellStyle name="通貨_Flat.File.Home.JP" xfId="412"/>
-    <cellStyle name="集計" xfId="413"/>
+    <cellStyle name="Zelle überprüfen" xfId="388" xr:uid="{00000000-0005-0000-0000-000085010000}"/>
+    <cellStyle name="アクセント 1" xfId="389" xr:uid="{00000000-0005-0000-0000-000086010000}"/>
+    <cellStyle name="アクセント 2" xfId="390" xr:uid="{00000000-0005-0000-0000-000087010000}"/>
+    <cellStyle name="アクセント 3" xfId="391" xr:uid="{00000000-0005-0000-0000-000088010000}"/>
+    <cellStyle name="アクセント 4" xfId="392" xr:uid="{00000000-0005-0000-0000-000089010000}"/>
+    <cellStyle name="アクセント 5" xfId="393" xr:uid="{00000000-0005-0000-0000-00008A010000}"/>
+    <cellStyle name="アクセント 6" xfId="394" xr:uid="{00000000-0005-0000-0000-00008B010000}"/>
+    <cellStyle name="タイトル" xfId="395" xr:uid="{00000000-0005-0000-0000-00008C010000}"/>
+    <cellStyle name="チェック セル" xfId="396" xr:uid="{00000000-0005-0000-0000-00008D010000}"/>
+    <cellStyle name="どちらでもない" xfId="397" xr:uid="{00000000-0005-0000-0000-00008E010000}"/>
+    <cellStyle name="メモ" xfId="398" xr:uid="{00000000-0005-0000-0000-00008F010000}"/>
+    <cellStyle name="リンク セル" xfId="399" xr:uid="{00000000-0005-0000-0000-000090010000}"/>
+    <cellStyle name="入力" xfId="400" xr:uid="{00000000-0005-0000-0000-000091010000}"/>
+    <cellStyle name="出力" xfId="401" xr:uid="{00000000-0005-0000-0000-000092010000}"/>
+    <cellStyle name="悪い" xfId="402" xr:uid="{00000000-0005-0000-0000-000093010000}"/>
+    <cellStyle name="標準_Data Definitions" xfId="403" xr:uid="{00000000-0005-0000-0000-000094010000}"/>
+    <cellStyle name="良い" xfId="404" xr:uid="{00000000-0005-0000-0000-000095010000}"/>
+    <cellStyle name="見出し 1" xfId="405" xr:uid="{00000000-0005-0000-0000-000096010000}"/>
+    <cellStyle name="見出し 2" xfId="406" xr:uid="{00000000-0005-0000-0000-000097010000}"/>
+    <cellStyle name="見出し 3" xfId="407" xr:uid="{00000000-0005-0000-0000-000098010000}"/>
+    <cellStyle name="見出し 4" xfId="408" xr:uid="{00000000-0005-0000-0000-000099010000}"/>
+    <cellStyle name="計算" xfId="409" xr:uid="{00000000-0005-0000-0000-00009A010000}"/>
+    <cellStyle name="説明文" xfId="410" xr:uid="{00000000-0005-0000-0000-00009B010000}"/>
+    <cellStyle name="警告文" xfId="411" xr:uid="{00000000-0005-0000-0000-00009C010000}"/>
+    <cellStyle name="通貨_Flat.File.Home.JP" xfId="412" xr:uid="{00000000-0005-0000-0000-00009D010000}"/>
+    <cellStyle name="集計" xfId="413" xr:uid="{00000000-0005-0000-0000-00009E010000}"/>
   </cellStyles>
   <dxfs count="85">
     <dxf>
@@ -5804,7 +5805,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -6122,7 +6129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
@@ -6441,9 +6448,9 @@
     <mergeCell ref="A21:B22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A25" r:id="rId1"/>
-    <hyperlink ref="A21" r:id="rId2" display="Email changes to aws-marketplace-seller-ops@amazon.com"/>
-    <hyperlink ref="A21:B22" r:id="rId3" display="●   Please submit completed forms via the File Upload tab of the AWS Marketplace Management Portal, https://aws.amazon.com/marketplace/management/"/>
+    <hyperlink ref="A25" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A21" r:id="rId2" display="Email changes to aws-marketplace-seller-ops@amazon.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A21:B22" r:id="rId3" display="●   Please submit completed forms via the File Upload tab of the AWS Marketplace Management Portal, https://aws.amazon.com/marketplace/management/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="8" orientation="portrait" r:id="rId4"/>
@@ -6456,15 +6463,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:JU11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15.95" customHeight="1"/>
@@ -7460,7 +7467,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="2" spans="1:281" s="99" customFormat="1" ht="36">
+    <row r="2" spans="1:281" s="99" customFormat="1" ht="36" hidden="1">
       <c r="A2" s="91"/>
       <c r="B2" s="92"/>
       <c r="C2" s="92"/>
@@ -8095,7 +8102,7 @@
       <c r="IV2" s="233"/>
       <c r="JU2" s="238"/>
     </row>
-    <row r="3" spans="1:281" s="21" customFormat="1" ht="12">
+    <row r="3" spans="1:281" s="21" customFormat="1" ht="12" hidden="1">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -8730,7 +8737,7 @@
       <c r="IV3" s="234"/>
       <c r="JU3" s="239"/>
     </row>
-    <row r="4" spans="1:281" s="21" customFormat="1" ht="12">
+    <row r="4" spans="1:281" s="21" customFormat="1" ht="12" hidden="1">
       <c r="A4" s="18"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -14435,7 +14442,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="11" spans="1:281" ht="409.5">
+    <row r="11" spans="1:281" ht="123" customHeight="1">
       <c r="A11" s="29" t="s">
         <v>501</v>
       </c>
@@ -15281,7 +15288,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:JH5"/>
+  <autoFilter ref="A5:JH5" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataConsolidate/>
   <conditionalFormatting sqref="Z6:AA6">
     <cfRule type="expression" dxfId="84" priority="83">
@@ -15679,270 +15686,270 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="634" yWindow="517" count="88">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Product Category 1" prompt="Primary Category for your product, selected from the drop-down list of valid categories. _x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="I5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Type" prompt="The fullfillment type for the product; SaaS (Software as a Service) or AMI (Amazon Machine Image)._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="Y5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Architecture" prompt="32-bit or 64-bit software architecture._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AD5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Operating System" prompt="Enter the OS of the product from the list of supported Operating Systems._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AE5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future domestic (US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BF5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future international (non-US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BG5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Recommended Instance Type" prompt="Choose the default instance type the product will use with 1-Click launch._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BH5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="FUTURE instance types" prompt="Make the product available in future instance types (non-paid products, depending on architecture)? Marketplace will automatically add to any new instance types._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BI5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Pricing Model" prompt="Select the pricing model for the software charges for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="DQ5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Only TRUE or FALSE values are allowed.  Please try again." promptTitle="Support Offered" prompt="Define if support (of any kind) is offered for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="U5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Virtualization" prompt="For Linux-based AMIs, is the virtualization HVM (hardware virtual machine) or PV (paravirtual)?  Windows-based AMIs are HVM._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AC5"/>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="Make product available on specific instance type._x000a__x000a_NOTE: All virtualization types and architecture are NOT supported on all instance types.  Please check the notes above or the Seller Guide for more information._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="IF5:II5 FX5:GA5 BJ5:DP5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement in which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IV5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement on which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IW5"/>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 15 characters.  Please try again." promptTitle="Flexible Consumption Pricing" prompt="The name used when sending metering records by calling MeterUsage API. Visible in billing reports. Does not need to be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 15 character MAX_x000a_* Alphanumeric and underscore only" sqref="IX6 JA6 JD6 JG6 JJ6 JM6 JP6 JS6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Product Category 1" prompt="Primary Category for your product, selected from the drop-down list of valid categories. _x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="I5" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Type" prompt="The fullfillment type for the product; SaaS (Software as a Service) or AMI (Amazon Machine Image)._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="Y5" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Architecture" prompt="32-bit or 64-bit software architecture._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AD5" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Operating System" prompt="Enter the OS of the product from the list of supported Operating Systems._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AE5" xr:uid="{00000000-0002-0000-0100-000003000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future domestic (US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BF5" xr:uid="{00000000-0002-0000-0100-000004000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future international (non-US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BG5" xr:uid="{00000000-0002-0000-0100-000005000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Recommended Instance Type" prompt="Choose the default instance type the product will use with 1-Click launch._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BH5" xr:uid="{00000000-0002-0000-0100-000006000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="FUTURE instance types" prompt="Make the product available in future instance types (non-paid products, depending on architecture)? Marketplace will automatically add to any new instance types._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BI5" xr:uid="{00000000-0002-0000-0100-000007000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Pricing Model" prompt="Select the pricing model for the software charges for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="DQ5" xr:uid="{00000000-0002-0000-0100-000008000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Only TRUE or FALSE values are allowed.  Please try again." promptTitle="Support Offered" prompt="Define if support (of any kind) is offered for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="U5" xr:uid="{00000000-0002-0000-0100-000009000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Virtualization" prompt="For Linux-based AMIs, is the virtualization HVM (hardware virtual machine) or PV (paravirtual)?  Windows-based AMIs are HVM._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AC5" xr:uid="{00000000-0002-0000-0100-00000A000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="Make product available on specific instance type._x000a__x000a_NOTE: All virtualization types and architecture are NOT supported on all instance types.  Please check the notes above or the Seller Guide for more information._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="IF5:II5 FX5:GA5 BJ5:DP5" xr:uid="{00000000-0002-0000-0100-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement in which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IV5" xr:uid="{00000000-0002-0000-0100-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement on which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IW5" xr:uid="{00000000-0002-0000-0100-00000D000000}"/>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 15 characters.  Please try again." promptTitle="Flexible Consumption Pricing" prompt="The name used when sending metering records by calling MeterUsage API. Visible in billing reports. Does not need to be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 15 character MAX_x000a_* Alphanumeric and underscore only" sqref="IX6 JA6 JD6 JG6 JJ6 JM6 JP6 JS6" xr:uid="{00000000-0002-0000-0100-00000E000000}">
       <formula1>1</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement in which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IV6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement in which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IV6" xr:uid="{00000000-0002-0000-0100-00000F000000}">
       <formula1>FCP_Category</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a decimal &gt;= 0.000.  Please try again." promptTitle="Flexible Consumption Pricing" prompt="The SOFTWARE charge per FCP Unit for this product._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.000" sqref="IZ6 JC6 JF6 JI6 JL6 JO6 JR6 JU6">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a decimal &gt;= 0.000.  Please try again." promptTitle="Flexible Consumption Pricing" prompt="The SOFTWARE charge per FCP Unit for this product._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.000" sqref="IZ6 JC6 JF6 JI6 JL6 JO6 JR6 JU6" xr:uid="{00000000-0002-0000-0100-000010000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The customer facing statement that describes the dimension for the product. Should be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 70 character MAX_x000a__x000a_EXAMPLES:_x000a_* Administrators per hour_x000a_* Per Mbps Bandwidth provisioned " sqref="JB5 IY5 JE5 JH5 JK5 JN5 JQ5 JT5"/>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Software by" prompt="ISV, company name or developer of the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="B5:B6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The customer facing statement that describes the dimension for the product. Should be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 70 character MAX_x000a__x000a_EXAMPLES:_x000a_* Administrators per hour_x000a_* Per Mbps Bandwidth provisioned " sqref="JB5 IY5 JE5 JH5 JK5 JN5 JQ5 JT5" xr:uid="{00000000-0002-0000-0100-000011000000}"/>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Software by" prompt="ISV, company name or developer of the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="B5:B6" xr:uid="{00000000-0002-0000-0100-000012000000}">
       <formula1>AND(LEN(B5)&gt;=1,LEN(B5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Title" prompt="Name of the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="C5:C6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Title" prompt="Name of the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="C5:C6" xr:uid="{00000000-0002-0000-0100-000013000000}">
       <formula1>AND(LEN(C5)&gt;=1,LEN(C5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 300 characters.  Please try again." promptTitle="Short Description" prompt="Short description of the product, used in AWS Marketplace on EC2 Console._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 300 character MAX" sqref="D5:D6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 300 characters.  Please try again." promptTitle="Short Description" prompt="Short description of the product, used in AWS Marketplace on EC2 Console._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 300 character MAX" sqref="D5:D6" xr:uid="{00000000-0002-0000-0100-000014000000}">
       <formula1>AND(LEN(D5)&gt;=1,LEN(D5)&lt;=300)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 1500 characters.  Please try again." promptTitle="Full Description" prompt="Description of the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 1500 character MAX" sqref="E5:E6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 1500 characters.  Please try again." promptTitle="Full Description" prompt="Description of the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 1500 character MAX" sqref="E5:E6" xr:uid="{00000000-0002-0000-0100-000015000000}">
       <formula1>AND(LEN(E5)&gt;=1,LEN(E5)&lt;=1500)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 250 characters.  Please try again." promptTitle="Highlight1" prompt="Short bullet-style callout of a key product feature._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 250 character MAX" sqref="F5:F6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 250 characters.  Please try again." promptTitle="Highlight1" prompt="Short bullet-style callout of a key product feature._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 250 character MAX" sqref="F5:F6" xr:uid="{00000000-0002-0000-0100-000016000000}">
       <formula1>AND(LEN(F5)&gt;=1,LEN(F5)&lt;=250)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no longer than 250 characters.  Please try again." promptTitle="Highlight2" prompt="Short bullet-style callout of a key product feature._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 250 character MAX" sqref="G5:G6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no longer than 250 characters.  Please try again." promptTitle="Highlight2" prompt="Short bullet-style callout of a key product feature._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 250 character MAX" sqref="G5:G6" xr:uid="{00000000-0002-0000-0100-000017000000}">
       <formula1>LEN(G5)&lt;=250</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no longer than 250 characters.  Please try again." promptTitle="Highlight3" prompt="Short bullet-style callout of a key product feature._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 250 character MAX" sqref="H5:H6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no longer than 250 characters.  Please try again." promptTitle="Highlight3" prompt="Short bullet-style callout of a key product feature._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 250 character MAX" sqref="H5:H6" xr:uid="{00000000-0002-0000-0100-000018000000}">
       <formula1>LEN(H5)&lt;=250</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Product Category 1" prompt="Primary Category for your product, selected from the drop-down list of valid categories. _x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="I6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Product Category 1" prompt="Primary Category for your product, selected from the drop-down list of valid categories. _x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="I6" xr:uid="{00000000-0002-0000-0100-000019000000}">
       <formula1>Category</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no greater than 72 characters.  Please try again." promptTitle="Product Category2" prompt="Enter an additional Marketplace Category, or an extra product keyword for search and browse._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="J5:J6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no greater than 72 characters.  Please try again." promptTitle="Product Category2" prompt="Enter an additional Marketplace Category, or an extra product keyword for search and browse._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="J5:J6" xr:uid="{00000000-0002-0000-0100-00001A000000}">
       <formula1>LEN(J5)&lt;=72</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no greater than 72 characters.  Please try again." promptTitle="Product Category3" prompt="Enter an additional Marketplace Category, or an extra product keyword for search and browse._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="K5:K6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be no greater than 72 characters.  Please try again." promptTitle="Product Category3" prompt="Enter an additional Marketplace Category, or an extra product keyword for search and browse._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="K5:K6" xr:uid="{00000000-0002-0000-0100-00001B000000}">
       <formula1>LEN(K5)&lt;=72</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Resource1_Name" prompt="Name of an additional resource for learning about the product (product sheets, white papers).  Displayed as the text for corresponding hyperlink._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX" sqref="M5:M6">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Resource1_Name" prompt="Name of an additional resource for learning about the product (product sheets, white papers).  Displayed as the text for corresponding hyperlink._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX" sqref="M5:M6" xr:uid="{00000000-0002-0000-0100-00001C000000}">
       <formula1>AND(LEN(M5)&gt;=1,LEN(M5)&lt;=50)</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Resource1_URL" prompt="URL for the Resource1_Name_x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="N5:N6">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Resource1_URL" prompt="URL for the Resource1_Name_x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="N5:N6" xr:uid="{00000000-0002-0000-0100-00001D000000}">
       <formula1>UPPER(LEFT(N5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Resource2_Name" prompt="Name of an additional resource for learning about the product (product sheets, white papers).  Displayed as the text for corresponding hyperlink._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX" sqref="O5:O6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Resource2_Name" prompt="Name of an additional resource for learning about the product (product sheets, white papers).  Displayed as the text for corresponding hyperlink._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX" sqref="O5:O6" xr:uid="{00000000-0002-0000-0100-00001E000000}">
       <formula1>AND(LEN(O5)&gt;=1,LEN(O5)&lt;=50)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Resource2_URL" prompt="URL for the Resource2_Name_x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="P5:P6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Resource2_URL" prompt="URL for the Resource2_Name_x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="P5:P6" xr:uid="{00000000-0002-0000-0100-00001F000000}">
       <formula1>UPPER(LEFT(P5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Resource3_Name" prompt="Name of an additional resource for learning about the product (product sheets, white papers).  Displayed as the text for corresponding hyperlink._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX" sqref="Q5:Q6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Resource3_Name" prompt="Name of an additional resource for learning about the product (product sheets, white papers).  Displayed as the text for corresponding hyperlink._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX" sqref="Q5:Q6" xr:uid="{00000000-0002-0000-0100-000020000000}">
       <formula1>AND(LEN(Q5)&gt;=1,LEN(Q5)&lt;=50)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Resource3_URL" prompt="URL for the Resource3_Name_x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="R5:R6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Resource3_URL" prompt="URL for the Resource3_Name_x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="R5:R6" xr:uid="{00000000-0002-0000-0100-000021000000}">
       <formula1>UPPER(LEFT(R5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Image URL" prompt="Enter the URL for the product image. Title treatments and logos display better than text-based._x000a__x000a_SPECIFICATIONS:_x000a_* Between 2:1 to 1:1 aspect ratio_x000a_* At least 110 pixels on the longest side_x000a_* png or jpg format" sqref="S5:S6">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Image URL" prompt="Enter the URL for the product image. Title treatments and logos display better than text-based._x000a__x000a_SPECIFICATIONS:_x000a_* Between 2:1 to 1:1 aspect ratio_x000a_* At least 110 pixels on the longest side_x000a_* png or jpg format" sqref="S5:S6" xr:uid="{00000000-0002-0000-0100-000022000000}">
       <formula1>UPPER(LEFT(S5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Product Video" prompt="URL for a video for your product, shown as the &quot;See product video&quot; link at the top of the product page._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="T5:T6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Product Video" prompt="URL for a video for your product, shown as the &quot;See product video&quot; link at the top of the product page._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="T5:T6" xr:uid="{00000000-0002-0000-0100-000023000000}">
       <formula1>UPPER(LEFT(T5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Support Contacts" prompt="Contact information, phone numbers and URLs to reach the support group for the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="V5:V6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Support Contacts" prompt="Contact information, phone numbers and URLs to reach the support group for the product._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="V5:V6" xr:uid="{00000000-0002-0000-0100-000024000000}">
       <formula1>AND(LEN(V5)&gt;=1,LEN(V5)&lt;=500)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Support Description" prompt="Describes the type of support offered._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="W5:W6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Support Description" prompt="Describes the type of support offered._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="W5:W6" xr:uid="{00000000-0002-0000-0100-000025000000}">
       <formula1>AND(LEN(W5)&gt;=1,LEN(W5)&lt;=500)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Type" prompt="The fullfillment type for the product; SaaS (Software as a Service) or AMI (Amazon Machine Image)._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="Y6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Type" prompt="The fullfillment type for the product; SaaS (Software as a Service) or AMI (Amazon Machine Image)._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="Y6" xr:uid="{00000000-0002-0000-0100-000026000000}">
       <formula1>Product_Type</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 250 characters.  Please try again." promptTitle="SaaS Pricing" prompt="Format: &quot;From $X per Y&quot; where X is the starting price (or range) and Y is a paramater such as hour/month/user. Must be in USD but can include local currency._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 250 character MAX" sqref="AA5:AA6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 250 characters.  Please try again." promptTitle="SaaS Pricing" prompt="Format: &quot;From $X per Y&quot; where X is the starting price (or range) and Y is a paramater such as hour/month/user. Must be in USD but can include local currency._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 250 character MAX" sqref="AA5:AA6" xr:uid="{00000000-0002-0000-0100-000027000000}">
       <formula1>LEN(AA5)&lt;=250</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 12 characters.  Please try again." promptTitle="&quot;Source&quot; AMI ID" prompt="Enter the AMI ID of the source AMI in the us-east-1 region, properly shared with our Marketplace account.  The source ami will be cloned to all regions by Marketplace._x000a__x000a_SPECIFICATIONS:_x000a_* format = ami-xxxxxxxx_x000a_* 12 character MAX_x000a_" sqref="AB5:AB6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 12 characters.  Please try again." promptTitle="&quot;Source&quot; AMI ID" prompt="Enter the AMI ID of the source AMI in the us-east-1 region, properly shared with our Marketplace account.  The source ami will be cloned to all regions by Marketplace._x000a__x000a_SPECIFICATIONS:_x000a_* format = ami-xxxxxxxx_x000a_* 12 character MAX_x000a_" sqref="AB5:AB6" xr:uid="{00000000-0002-0000-0100-000028000000}">
       <formula1>AND(LEN(AB5)&gt;=1,LEN(AB5)&lt;=12)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Architecture" prompt="32-bit or 64-bit software architecture._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AD6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Architecture" prompt="32-bit or 64-bit software architecture._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AD6" xr:uid="{00000000-0002-0000-0100-000029000000}">
       <formula1>Architecture</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Operating System" prompt="Enter the OS of the product from the list of supported Operating Systems._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AE6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Operating System" prompt="Enter the OS of the product from the list of supported Operating Systems._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AE6" xr:uid="{00000000-0002-0000-0100-00002A000000}">
       <formula1>Operating_System</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Operating System Version" prompt="Enter the specific version of the Operating System._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="AF5:AF6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Operating System Version" prompt="Enter the specific version of the Operating System._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="AF5:AF6" xr:uid="{00000000-0002-0000-0100-00002B000000}">
       <formula1>AND(LEN(AF5)&gt;=1,LEN(AF5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Operating System login username" prompt="Enter the login username used to access the OS; i.e. ec2-user, ubuntu, Administrator._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="AG5:AG6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Operating System login username" prompt="Enter the login username used to access the OS; i.e. ec2-user, ubuntu, Administrator._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="AG5:AG6" xr:uid="{00000000-0002-0000-0100-00002C000000}">
       <formula1>AND(LEN(AG5)&gt;=1,LEN(AG5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="PIOPS TOTAL" prompt="For pIOPS products, the total PIOPS across the entire product, all connections._x000a__x000a_SPECIFICATIONS:_x000a_* Integer" sqref="AH5:AH6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="PIOPS TOTAL" prompt="For pIOPS products, the total PIOPS across the entire product, all connections._x000a__x000a_SPECIFICATIONS:_x000a_* Integer" sqref="AH5:AH6" xr:uid="{00000000-0002-0000-0100-00002D000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="AWS Services Required" prompt="List all AWS services that are required for the product to function correctly.  i.e. EC2, EBS, S3_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 150 character MAX" sqref="AI5:AI6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="AWS Services Required" prompt="List all AWS services that are required for the product to function correctly.  i.e. EC2, EBS, S3_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 150 character MAX" sqref="AI5:AI6" xr:uid="{00000000-0002-0000-0100-00002E000000}">
       <formula1>LEN(AI5)&lt;=72</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="3rd Party Software Included" prompt="A comma seprated list of any 3rd party software that is part of the AMI, including open source._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="AJ5:AJ6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="3rd Party Software Included" prompt="A comma seprated list of any 3rd party software that is part of the AMI, including open source._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="AJ5:AJ6" xr:uid="{00000000-0002-0000-0100-00002F000000}">
       <formula1>AND(LEN(AJ5)&gt;=1,LEN(AJ5)&lt;=500)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 36 characters.  Please try again." promptTitle="Version Title" prompt="The version name or title.  Ex: 1.2.6a, 2010SP1_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 36 character MAX" sqref="AK5:AK6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 36 characters.  Please try again." promptTitle="Version Title" prompt="The version name or title.  Ex: 1.2.6a, 2010SP1_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 36 character MAX" sqref="AK5:AK6" xr:uid="{00000000-0002-0000-0100-000030000000}">
       <formula1>AND(LEN(AK5)&gt;=1,LEN(AK5)&lt;=36)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Release Notes" prompt="Notes regarding changes in the newest version.  URLs are supported._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="AL5:AL6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Release Notes" prompt="Notes regarding changes in the newest version.  URLs are supported._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="AL5:AL6" xr:uid="{00000000-0002-0000-0100-000031000000}">
       <formula1>AND(LEN(AL5)&gt;=1,LEN(AL5)&lt;=500)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be less than 1500 characters.  Please try again." promptTitle="Instance Migration Instructions" prompt="Information on how an end-user can upgrade from one version of the product to another; i.e. how can they preserve data and settings when creating another instance._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1500 character MAX" sqref="AM5:AM6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be less than 1500 characters.  Please try again." promptTitle="Instance Migration Instructions" prompt="Information on how an end-user can upgrade from one version of the product to another; i.e. how can they preserve data and settings when creating another instance._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1500 character MAX" sqref="AM5:AM6" xr:uid="{00000000-0002-0000-0100-000032000000}">
       <formula1>AND(LEN(AM5)&lt;=1500)</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 1500 characters.  Please try again." promptTitle="Product Access Instructions" prompt="Step by step instructions for the end-user to launch, configure and access the product. Write with a less-technical customer in mind. Can include URL to more comprehensive steps._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1500 character MAX" sqref="AN5:AN6">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 1500 characters.  Please try again." promptTitle="Product Access Instructions" prompt="Step by step instructions for the end-user to launch, configure and access the product. Write with a less-technical customer in mind. Can include URL to more comprehensive steps._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1500 character MAX" sqref="AN5:AN6" xr:uid="{00000000-0002-0000-0100-000033000000}">
       <formula1>AND(LEN(AN5)&gt;=1,LEN(AN5)&lt;=1500)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Endpoint URL protocol" prompt="For products with a browser interface, enter the protocol portion of the endpoint &quot;http://&lt;Public_DNS&gt;/relative.htm:port&quot;; i.e. http, https._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AO5:AO6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Endpoint URL protocol" prompt="For products with a browser interface, enter the protocol portion of the endpoint &quot;http://&lt;Public_DNS&gt;/relative.htm:port&quot;; i.e. http, https._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AO5:AO6" xr:uid="{00000000-0002-0000-0100-000034000000}">
       <formula1>Endpoint_Protocol</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be an integer &lt;=65535.  Please try again." promptTitle="Endpoint URL port" prompt="For products with a browser interface, enter the port portion of the endpoint &quot;http://&lt;Public_DNS&gt;/relative.htm:port&quot;; i.e. 80, 443_x000a__x000a_SPECIFICATIONS:_x000a_* Integer" sqref="AP5:AP6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be an integer &lt;=65535.  Please try again." promptTitle="Endpoint URL port" prompt="For products with a browser interface, enter the port portion of the endpoint &quot;http://&lt;Public_DNS&gt;/relative.htm:port&quot;; i.e. 80, 443_x000a__x000a_SPECIFICATIONS:_x000a_* Integer" sqref="AP5:AP6" xr:uid="{00000000-0002-0000-0100-000035000000}">
       <formula1>1</formula1>
       <formula2>65535</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be less than 72 characters.  Please try again." promptTitle="Endpoint URL relative" prompt="For products with a browser interface, enter the relative URLportion of the endpoint &quot;http://&lt;Public_DNS&gt;/relative.htm:port&quot;; i.e.index.html_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="AQ5:AQ6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be less than 72 characters.  Please try again." promptTitle="Endpoint URL relative" prompt="For products with a browser interface, enter the relative URLportion of the endpoint &quot;http://&lt;Public_DNS&gt;/relative.htm:port&quot;; i.e.index.html_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="AQ5:AQ6" xr:uid="{00000000-0002-0000-0100-000036000000}">
       <formula1>AND(LEN(AQ5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="EULA" prompt="Enter the URL for the End User License Agreement for the product._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL_x000a_" sqref="AR5:AR6">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="EULA" prompt="Enter the URL for the End User License Agreement for the product._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL_x000a_" sqref="AR5:AR6" xr:uid="{00000000-0002-0000-0100-000037000000}">
       <formula1>UPPER(LEFT(AR5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be less than 72 characters.  Please try again." promptTitle="Fulfillment Title" prompt="For Cloud Formation deployment, enter a friendly name for the fullfillment method; i.e. Into custom VPC_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="AS5:AS6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be less than 72 characters.  Please try again." promptTitle="Fulfillment Title" prompt="For Cloud Formation deployment, enter a friendly name for the fullfillment method; i.e. Into custom VPC_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 72 character MAX" sqref="AS5:AS6" xr:uid="{00000000-0002-0000-0100-000038000000}">
       <formula1>AND(LEN(AS5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Cloud Formation Template URL" prompt="For VPC Cloud Formation deployment ONLY, enter the URL to the CF Template._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="AT5:AT6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="Cloud Formation Template URL" prompt="For VPC Cloud Formation deployment ONLY, enter the URL to the CF Template._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="AT5:AT6" xr:uid="{00000000-0002-0000-0100-000039000000}">
       <formula1>UPPER(LEFT(AT5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future domestic (US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BF6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future domestic (US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BF6" xr:uid="{00000000-0002-0000-0100-00003A000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future international (non-US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BG6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Make available in FUTURE regions" prompt="Make the product available in future international (non-US) EC2 regions? Marketplace will automatically add to any new regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BG6" xr:uid="{00000000-0002-0000-0100-00003B000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="FUTURE instance types" prompt="Make the product available in future instance types (non-paid products, depending on architecture)? Marketplace will automatically add to any new instance types._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BI6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="FUTURE instance types" prompt="Make the product available in future instance types (non-paid products, depending on architecture)? Marketplace will automatically add to any new instance types._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="BI6" xr:uid="{00000000-0002-0000-0100-00003C000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Pricing Model" prompt="Select the pricing model for the software charges for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="DQ6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Pricing Model" prompt="Select the pricing model for the software charges for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="DQ6" xr:uid="{00000000-0002-0000-0100-00003D000000}">
       <formula1>Pricing_Model</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be an integer &lt;=1.  Please try again." promptTitle="Free Trial Instance Count" prompt="For Free Trial enabled products, enter the number of instances the Free Trial should include.  Currently only 1 allowed_x000a__x000a_SPECIFICATIONS:_x000a_* integer between 1 and 1" sqref="DS5:DS6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be an integer &lt;=1.  Please try again." promptTitle="Free Trial Instance Count" prompt="For Free Trial enabled products, enter the number of instances the Free Trial should include.  Currently only 1 allowed_x000a__x000a_SPECIFICATIONS:_x000a_* integer between 1 and 1" sqref="DS5:DS6" xr:uid="{00000000-0002-0000-0100-00003E000000}">
       <formula1>1</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a decimal &gt;= 0.000.  Please try again." promptTitle="Hourly pricing for instance type" prompt="For paid products with an Hourly component, what is the SOFTWARE charge per hour for this instance type (AWS charges are computed separately)?  Precision is 3 decimal points; i.e. 2.100, 0.150._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.000" sqref="DU5:DU6 DV6 DW5:FW6">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a decimal &gt;= 0.000.  Please try again." promptTitle="Hourly pricing for instance type" prompt="For paid products with an Hourly component, what is the SOFTWARE charge per hour for this instance type (AWS charges are computed separately)?  Precision is 3 decimal points; i.e. 2.100, 0.150._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.000" sqref="DU5:DU6 DV6 DW5:FW6" xr:uid="{00000000-0002-0000-0100-00003F000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="SKU" prompt="Unique identifier for your product.  Must be unuique for each product listing.  Ex: CloudPower_0001_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="A5:A6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="SKU" prompt="Unique identifier for your product.  Must be unuique for each product listing.  Ex: CloudPower_0001_x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 72 character MAX" sqref="A5:A6" xr:uid="{00000000-0002-0000-0100-000040000000}">
       <formula1>AND(LEN(A5)&gt;=1,LEN(A5)&lt;=72)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Only TRUE or FALSE values are allowed.  Please try again." promptTitle="Support Offered" prompt="Define if support (of any kind) is offered for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="U6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Only TRUE or FALSE values are allowed.  Please try again." promptTitle="Support Offered" prompt="Define if support (of any kind) is offered for the product._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="U6" xr:uid="{00000000-0002-0000-0100-000041000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Search Keywords" prompt="Enter up to 50 characters of comma separated keywords._x000a__x000a_NOTE: Seller name, product name and all categories are automatically added as search keywords._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX_x000a_* comma separated" sqref="L5:L6">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 50 characters.  Please try again." promptTitle="Search Keywords" prompt="Enter up to 50 characters of comma separated keywords._x000a__x000a_NOTE: Seller name, product name and all categories are automatically added as search keywords._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 50 character MAX_x000a_* comma separated" sqref="L5:L6" xr:uid="{00000000-0002-0000-0100-000042000000}">
       <formula1>AND(LEN(L5)&gt;=1,LEN(L5)&lt;=50)</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Refund and Cancelation Policy" prompt="Describes the refund policy for software charges, even if the policy is &quot;no refunds&quot;.  It is highly encouraged to offer some form of refund and contact information._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="X5:X6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 500 characters.  Please try again." promptTitle="Refund and Cancelation Policy" prompt="Describes the refund policy for software charges, even if the policy is &quot;no refunds&quot;.  It is highly encouraged to offer some form of refund and contact information._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 1 character MIN_x000a_* 500 character MAX" sqref="X5:X6" xr:uid="{00000000-0002-0000-0100-000043000000}">
       <formula1>AND(LEN(X5)&gt;=1,LEN(X5)&lt;=500)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Value MUST be an integer &gt;=1 and &lt;= 31.  Please try again." promptTitle="Free Trial Duration" prompt="For Free Trial enabled products, enter the number days of the free trial._x000a__x000a_SPECIFICATIONS:_x000a_* integer between 5 and 31" sqref="DT5:DT6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Value MUST be an integer &gt;=1 and &lt;= 31.  Please try again." promptTitle="Free Trial Duration" prompt="For Free Trial enabled products, enter the number days of the free trial._x000a__x000a_SPECIFICATIONS:_x000a_* integer between 5 and 31" sqref="DT5:DT6" xr:uid="{00000000-0002-0000-0100-000044000000}">
       <formula1>5</formula1>
       <formula2>31</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="SaaS Product URL" prompt="URL for customer to visit to learn more about the SaaS product; acessed via the &quot;Visit Site&quot; button on the product page. _x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="Z5:Z6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="SaaS Product URL" prompt="URL for customer to visit to learn more about the SaaS product; acessed via the &quot;Visit Site&quot; button on the product page. _x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="Z5:Z6" xr:uid="{00000000-0002-0000-0100-000045000000}">
       <formula1>UPPER(LEFT(Z5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="Make product available on specific instance type._x000a__x000a_NOTE: All virtualization types and architecture are NOT supported on all instance types.  Please check the notes above or the Seller Guide for more information._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="IF6:II6 FX6:GA6 BJ6:DP6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="Make product available on specific instance type._x000a__x000a_NOTE: All virtualization types and architecture are NOT supported on all instance types.  Please check the notes above or the Seller Guide for more information._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="IF6:II6 FX6:GA6 BJ6:DP6" xr:uid="{00000000-0002-0000-0100-000046000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="BYOL URL" prompt="URL for customer to visit to obtain a BYOL license._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="DR5:DR6">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid URL" error="Must be a URL with http or https format." promptTitle="BYOL URL" prompt="URL for customer to visit to obtain a BYOL license._x000a__x000a_SPECIFICATIONS:_x000a_* Valid URL" sqref="DR5:DR6" xr:uid="{00000000-0002-0000-0100-000047000000}">
       <formula1>UPPER(LEFT(DR5,4)="http")</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a decimal &gt;= 0.00.  Please try again." promptTitle="Monthly pricing for product" prompt="For paid products with a Monthly software charge, the amount charged for software per month._x000a__x000a_NOTE: This is per subscription per month and does not impact nor is impacted by number or type of instances used._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.00" sqref="GB5:GB6">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a decimal &gt;= 0.00.  Please try again." promptTitle="Monthly pricing for product" prompt="For paid products with a Monthly software charge, the amount charged for software per month._x000a__x000a_NOTE: This is per subscription per month and does not impact nor is impacted by number or type of instances used._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.00" sqref="GB5:GB6" xr:uid="{00000000-0002-0000-0100-000048000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a whole number &gt; 0.  Please try again." promptTitle="Annual pricing for instance type" prompt="For paid products with an Annual pricing component, the amount charged for software per year per instancetype. Annual MUST include corresponding hourly rate.  Must be a whole number, &gt; 0; i.e. 2500, 12500._x000a__x000a_SPECIFICATIONS:_x000a_* Whole number_x000a_* &gt; 0" sqref="GC5:GC6 GD6 GE5:IE6">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD VALUE" error="Value MUST be a whole number &gt; 0.  Please try again." promptTitle="Annual pricing for instance type" prompt="For paid products with an Annual pricing component, the amount charged for software per year per instancetype. Annual MUST include corresponding hourly rate.  Must be a whole number, &gt; 0; i.e. 2500, 12500._x000a__x000a_SPECIFICATIONS:_x000a_* Whole number_x000a_* &gt; 0" sqref="GC5:GC6 GD6 GE5:IE6" xr:uid="{00000000-0002-0000-0100-000049000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Security Group / Ingress" prompt="Define a single ingress rule for the automatically created security group for the product. Follow the format: protocol, start_port, end_port, IP in CIDR. i.e. tcp,22,22,0.0.0.0/0_x000a__x000a_SPECIFICATIONS:_x000a_* protocol, start_port, end_port, IP in CIDR" sqref="IJ5:IU6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The name used when sending metering records by calling MeterUsage API. Visible in billing reports. Does not need to be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 15 character MAX_x000a_* Alphanumeric and underscore only" sqref="IX5 JA5 JD5 JG5 JJ5 JM5 JP5 JS5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The SOFTWARE charge per FCP Unit for this product._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.000" sqref="IZ5 JC5 JF5 JI5 JL5 JO5 JR5 JU5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The customer-facing statement that describes the dimension for the product. Visible in billing console. Should be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 70 character MAX_x000a__x000a_EXAMPLES:_x000a_* Administrators per hour_x000a_* Per Mbps Bandwidth provisioned " sqref="IY6 JE6 JH6 JK6 JN6 JQ6 JT6"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The customer-facing statement that describes the dimension for the product. Visible in billing console. Should be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 70 character MAX_x000a__x000a_EXAMPLES:_x000a_* Administrators per hour_x000a_* Per Mbps Bandwidth provisioned" sqref="JB6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement on which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IW6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="BAD LENGTH" error="Length MUST be between 1 and 72 characters.  Please try again." promptTitle="Security Group / Ingress" prompt="Define a single ingress rule for the automatically created security group for the product. Follow the format: protocol, start_port, end_port, IP in CIDR. i.e. tcp,22,22,0.0.0.0/0_x000a__x000a_SPECIFICATIONS:_x000a_* protocol, start_port, end_port, IP in CIDR" sqref="IJ5:IU6" xr:uid="{00000000-0002-0000-0100-00004A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The name used when sending metering records by calling MeterUsage API. Visible in billing reports. Does not need to be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 15 character MAX_x000a_* Alphanumeric and underscore only" sqref="IX5 JA5 JD5 JG5 JJ5 JM5 JP5 JS5" xr:uid="{00000000-0002-0000-0100-00004B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The SOFTWARE charge per FCP Unit for this product._x000a__x000a_SPECIFICATIONS:_x000a_* Decimal_x000a_* &gt;= 0.000" sqref="IZ5 JC5 JF5 JI5 JL5 JO5 JR5 JU5" xr:uid="{00000000-0002-0000-0100-00004C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The customer-facing statement that describes the dimension for the product. Visible in billing console. Should be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 70 character MAX_x000a__x000a_EXAMPLES:_x000a_* Administrators per hour_x000a_* Per Mbps Bandwidth provisioned " sqref="IY6 JE6 JH6 JK6 JN6 JQ6 JT6" xr:uid="{00000000-0002-0000-0100-00004D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The customer-facing statement that describes the dimension for the product. Visible in billing console. Should be user friendly._x000a__x000a_SPECIFICATIONS:_x000a_* Open text field_x000a_* 70 character MAX_x000a__x000a_EXAMPLES:_x000a_* Administrators per hour_x000a_* Per Mbps Bandwidth provisioned" sqref="JB6" xr:uid="{00000000-0002-0000-0100-00004E000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Flexible Consumption Pricing" prompt="The unit of measurement on which customers will be charged for paid products with a Usage pricing component._x000a__x000a_SPECIFICATIONS:_x000a_* List Selection" sqref="IW6" xr:uid="{00000000-0002-0000-0100-00004F000000}">
       <formula1>INDIRECT($IV6&amp;"_Units")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.large_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BW7:BW1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.large_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BW7:BW1048576" xr:uid="{00000000-0002-0000-0100-000050000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BX7:BX1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BX7:BX1048576" xr:uid="{00000000-0002-0000-0100-000051000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.2xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BY7:BY1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.2xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BY7:BY1048576" xr:uid="{00000000-0002-0000-0100-000052000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.4xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BZ7:BZ1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.4xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BZ7:BZ1048576" xr:uid="{00000000-0002-0000-0100-000053000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.10xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="CA7:CA1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_m4.10xlarge_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="CA7:CA1048576" xr:uid="{00000000-0002-0000-0100-000054000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_t2.large_x000a__x000a_Instance Limitations: HVM only_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BN7:BN1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Run on specific instance type" prompt="***REQUIRED***_x000a__x000a_Make product available on instance type._x000a__x000a_t2.large_x000a__x000a_Instance Limitations: HVM only_x000a__x000a_SPECIFICATIONS:_x000a_* List" sqref="BN7:BN1048576" xr:uid="{00000000-0002-0000-0100-000055000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Offered in specific EC2 region" prompt="Product offered in the EC2 region?  We reccomend making the product available in all regions when possible._x000a__x000a_NOTE: Marketplace clones a single source AMI to all regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AU5:BE5"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Offered in specific EC2 region" prompt="Product offered in the EC2 region?  We reccomend making the product available in all regions when possible._x000a__x000a_NOTE: Marketplace clones a single source AMI to all regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AU6:BE6">
+    <dataValidation showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Offered in specific EC2 region" prompt="Product offered in the EC2 region?  We reccomend making the product available in all regions when possible._x000a__x000a_NOTE: Marketplace clones a single source AMI to all regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AU5:BE5" xr:uid="{00000000-0002-0000-0100-000056000000}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Offered in specific EC2 region" prompt="Product offered in the EC2 region?  We reccomend making the product available in all regions when possible._x000a__x000a_NOTE: Marketplace clones a single source AMI to all regions._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" sqref="AU6:BE6" xr:uid="{00000000-0002-0000-0100-000057000000}">
       <formula1>TRUE_FALSE</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="AR6" r:id="rId1"/>
-    <hyperlink ref="R6" r:id="rId2"/>
-    <hyperlink ref="N6" r:id="rId3"/>
-    <hyperlink ref="P6" r:id="rId4"/>
-    <hyperlink ref="S6" r:id="rId5"/>
-    <hyperlink ref="T6" r:id="rId6"/>
-    <hyperlink ref="V6" r:id="rId7"/>
-    <hyperlink ref="W9" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo"/>
-    <hyperlink ref="W10" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo"/>
-    <hyperlink ref="W11" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo"/>
+    <hyperlink ref="AR6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="R6" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="N6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="P6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="S6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="T6" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="V6" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="W9" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="W10" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="W11" display="http://www.lansa.com/support/register/helpdesk.htm_x000a_The LANSA Product Support team is highly qualified to provide timely, accurate information and assistance on the entire suite of LANSA products. From answering simple installation questions to troubleshoo" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="634" yWindow="517" count="4">
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Recommended Instance Type" prompt="Choose the default instance type the product will use with 1-Click launch._x000a__x000a_SPECIFICATIONS:_x000a_* List selection">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Recommended Instance Type" prompt="Choose the default instance type the product will use with 1-Click launch._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" xr:uid="{00000000-0002-0000-0100-000058000000}">
           <x14:formula1>
             <xm:f>Validation_Data!$C$2:$C$55</xm:f>
           </x14:formula1>
           <xm:sqref>BH6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Virtualization" prompt="For Linux-based AMIs, is the virtualization HVM (hardware virtual machine) or PV (paravirtual)?  Windows-based AMIs are HVM._x000a__x000a_SPECIFICATIONS:_x000a_* List selection">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Virtualization" prompt="For Linux-based AMIs, is the virtualization HVM (hardware virtual machine) or PV (paravirtual)?  Windows-based AMIs are HVM._x000a__x000a_SPECIFICATIONS:_x000a_* List selection" xr:uid="{00000000-0002-0000-0100-000059000000}">
           <x14:formula1>
             <xm:f>Validation_Data!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>AC6</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Virtualization" prompt="***REQUIRED***_x000a__x000a_The AMI is HVM (hardware virtual machine) or PV (paravirtual)._x000a__x000a_SPECIFICATIONS:_x000a_* List">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Virtualization" prompt="***REQUIRED***_x000a__x000a_The AMI is HVM (hardware virtual machine) or PV (paravirtual)._x000a__x000a_SPECIFICATIONS:_x000a_* List" xr:uid="{00000000-0002-0000-0100-00005A000000}">
           <x14:formula1>
             <xm:f>Validation_Data!$J$2:$J$3</xm:f>
           </x14:formula1>
           <xm:sqref>AC7:AC1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Recommended Instance Type" prompt="***REQUIRED***_x000a__x000a_Choose the default instance type the product will use with 1-Click launch._x000a__x000a_SPECIFICATIONS:_x000a_* List">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="INVALID Selection" error="You have made an invalid selection, please select 1 item from the drop-down list." promptTitle="Recommended Instance Type" prompt="***REQUIRED***_x000a__x000a_Choose the default instance type the product will use with 1-Click launch._x000a__x000a_SPECIFICATIONS:_x000a_* List" xr:uid="{00000000-0002-0000-0100-00005B000000}">
           <x14:formula1>
             <xm:f>Validation_Data!$C$2:$C$55</xm:f>
           </x14:formula1>
@@ -15955,7 +15962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
@@ -16734,6 +16741,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AD819919D14AE4FA932A964A2021B57" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8237a4f1107e5ea924e50b28ebb65745">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -16847,33 +16869,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8353043-E31E-42E6-ADD1-2DF7C1AB4A57}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B5DC2E0-0871-44B1-89B4-ACA1409A331A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16894,9 +16893,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B5DC2E0-0871-44B1-89B4-ACA1409A331A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8353043-E31E-42E6-ADD1-2DF7C1AB4A57}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>